<commit_message>
add functionality to send attachmet from public url (internet)
</commit_message>
<xml_diff>
--- a/message.xlsx
+++ b/message.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t xml:space="preserve">nomer</t>
   </si>
@@ -34,102 +34,25 @@
     <t xml:space="preserve">attachment</t>
   </si>
   <si>
-    <t xml:space="preserve">628909899989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pesan dari excel tanpa gambar</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/gambar/tes.png</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/gambar/tes.pdf</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/gambar/tes.doc</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/gambar/tes.xls</t>
-    </r>
+    <t xml:space="preserve">url_public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6285599999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pesan dari excel dengan attachment dari local disk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/data/docker/wa-broadcast/unduhan/dicoding-logo-full.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pesan dari excel tanpa attachment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pesan dari excel gambar dari internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://asligresik.files.wordpress.com/2020/06/screenshot-from-2020-06-07-14-07-47.png</t>
   </si>
 </sst>
 </file>
@@ -240,17 +163,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.45"/>
@@ -271,92 +194,90 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">CONCATENATE(A2,"@c.us")</f>
-        <v>628909899989@c.us</v>
+        <v>6285599999999@c.us</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">CONCATENATE(A3,"@c.us")</f>
-        <v>628909899989@c.us</v>
+        <v>6285599999999@c.us</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">CONCATENATE(A4,"@c.us")</f>
-        <v>628909899989@c.us</v>
+        <v>6285599999999@c.us</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="0" t="str">
         <f aca="false">CONCATENATE(A5,"@c.us")</f>
-        <v>628909899989@c.us</v>
+        <v>6285599999999@c.us</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="str">
         <f aca="false">CONCATENATE(A6,"@c.us")</f>
-        <v>628909899989@c.us</v>
+        <v>6285599999999@c.us</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="0" t="str">
         <f aca="false">CONCATENATE(A7,"@c.us")</f>
-        <v>628909899989@c.us</v>
+        <v>6285599999999@c.us</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>